<commit_message>
ironing, cleaning up code
</commit_message>
<xml_diff>
--- a/comparison.xlsx
+++ b/comparison.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="45">
   <si>
     <t>C</t>
   </si>
@@ -132,9 +132,6 @@
     <t>comment</t>
   </si>
   <si>
-    <t>ASCII new page</t>
-  </si>
-  <si>
     <t>ORIGINAL</t>
   </si>
   <si>
@@ -151,6 +148,12 @@
   </si>
   <si>
     <t>space</t>
+  </si>
+  <si>
+    <t>size of data subblock</t>
+  </si>
+  <si>
+    <t>img!</t>
   </si>
 </sst>
 </file>
@@ -579,8 +582,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D54"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -593,16 +596,16 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>40</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -834,6 +837,9 @@
       <c r="B20">
         <v>255</v>
       </c>
+      <c r="C20">
+        <v>255</v>
+      </c>
       <c r="D20" s="4" t="s">
         <v>33</v>
       </c>
@@ -868,7 +874,7 @@
         <v>12</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
     </row>
     <row r="24" spans="1:4">
@@ -934,7 +940,7 @@
         <v>32</v>
       </c>
       <c r="D29" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="30" spans="1:4">
@@ -1011,7 +1017,7 @@
         <v>0</v>
       </c>
       <c r="D36" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="37" spans="1:4">
@@ -1022,6 +1028,9 @@
         <v>44</v>
       </c>
       <c r="C37">
+        <v>44</v>
+      </c>
+      <c r="D37" s="4" t="s">
         <v>44</v>
       </c>
     </row>

</xml_diff>

<commit_message>
reorganized, exposed final api
only (gif-write-images x) remains, as well as unrecognized GCE bug
</commit_message>
<xml_diff>
--- a/comparison.xlsx
+++ b/comparison.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="51">
   <si>
     <t>C</t>
   </si>
@@ -154,6 +154,24 @@
   </si>
   <si>
     <t>img!</t>
+  </si>
+  <si>
+    <t>G</t>
+  </si>
+  <si>
+    <t>I</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>width:</t>
+  </si>
+  <si>
+    <t>height:</t>
+  </si>
+  <si>
+    <t>trailer</t>
   </si>
 </sst>
 </file>
@@ -582,8 +600,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D54"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="J57" sqref="J57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -618,6 +636,9 @@
       <c r="C2">
         <v>71</v>
       </c>
+      <c r="D2" s="4" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="1">
@@ -629,6 +650,9 @@
       <c r="C3">
         <v>73</v>
       </c>
+      <c r="D3" s="4" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="1">
@@ -640,6 +664,9 @@
       <c r="C4">
         <v>70</v>
       </c>
+      <c r="D4" s="4" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="1">
@@ -651,6 +678,9 @@
       <c r="C5">
         <v>56</v>
       </c>
+      <c r="D5" s="4">
+        <v>8</v>
+      </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="1">
@@ -662,6 +692,9 @@
       <c r="C6">
         <v>57</v>
       </c>
+      <c r="D6" s="4">
+        <v>9</v>
+      </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" s="1">
@@ -673,6 +706,9 @@
       <c r="C7">
         <v>97</v>
       </c>
+      <c r="D7" s="4" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" s="1">
@@ -684,6 +720,9 @@
       <c r="C8">
         <v>3</v>
       </c>
+      <c r="D8" s="4" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" s="1">
@@ -695,6 +734,9 @@
       <c r="C9">
         <v>0</v>
       </c>
+      <c r="D9" s="4">
+        <v>3</v>
+      </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" s="1">
@@ -706,6 +748,9 @@
       <c r="C10">
         <v>3</v>
       </c>
+      <c r="D10" s="4" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" s="1">
@@ -717,6 +762,9 @@
       <c r="C11">
         <v>0</v>
       </c>
+      <c r="D11" s="4">
+        <v>3</v>
+      </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" s="1" t="s">
@@ -1155,7 +1203,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="49" spans="1:3">
+    <row r="49" spans="1:4">
       <c r="A49" s="1" t="s">
         <v>25</v>
       </c>
@@ -1166,7 +1214,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="50" spans="1:3">
+    <row r="50" spans="1:4">
       <c r="A50" s="1">
         <v>30</v>
       </c>
@@ -1177,7 +1225,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="51" spans="1:3">
+    <row r="51" spans="1:4">
       <c r="A51" s="1">
         <v>31</v>
       </c>
@@ -1188,7 +1236,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="52" spans="1:3">
+    <row r="52" spans="1:4">
       <c r="A52" s="1">
         <v>32</v>
       </c>
@@ -1199,7 +1247,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="53" spans="1:3">
+    <row r="53" spans="1:4">
       <c r="A53" s="1">
         <v>33</v>
       </c>
@@ -1210,7 +1258,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:3">
+    <row r="54" spans="1:4">
       <c r="A54" s="1">
         <v>34</v>
       </c>
@@ -1219,6 +1267,9 @@
       </c>
       <c r="C54">
         <v>59</v>
+      </c>
+      <c r="D54" s="4" t="s">
+        <v>50</v>
       </c>
     </row>
   </sheetData>

</xml_diff>